<commit_message>
ekec + chem masters paths updated
</commit_message>
<xml_diff>
--- a/Datasets/UCD_EngArch_Path_Chemical_ME_Modules.xlsx
+++ b/Datasets/UCD_EngArch_Path_Chemical_ME_Modules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alanh\Documents\GitHub\ChatGPTAssessment\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45FA0EF3-C88B-4C87-B8D7-43016C3BE8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026ECED4-E652-42A6-A260-8768550A8781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C7146B4A-4439-46E0-B60E-DB05B9DBCCC1}"/>
   </bookViews>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470AD8BE-D0F1-4863-8083-BF0D6224CD04}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43:C49"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>